<commit_message>
Aggregations of the results completed
</commit_message>
<xml_diff>
--- a/data/FA-SALES-Nov-20.xlsx
+++ b/data/FA-SALES-Nov-20.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University of Colorado\Subjects\Projects\gst_reco_tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73AC8C0A-76BA-425A-ACB9-2A31A3623C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8689D3F-E095-4831-9FBC-387FD15502E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Purchase Register" sheetId="1" r:id="rId1"/>
@@ -118,12 +118,6 @@
     <t>37AARFB6354R1ZH</t>
   </si>
   <si>
-    <t>BILL NO.MCCRS20/1375</t>
-  </si>
-  <si>
-    <t>BILL NO.MCCRS20/1366</t>
-  </si>
-  <si>
     <t>Saajan Youth Fashions, Vijayawada</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>BILL NO.SWCRS20/524</t>
   </si>
   <si>
-    <t>BILL NO.M1CRS20/387</t>
-  </si>
-  <si>
     <t>bill no.201100716</t>
   </si>
   <si>
@@ -172,15 +163,6 @@
     <t>BILL NO.BCRS20/651</t>
   </si>
   <si>
-    <t>BILL NO.MCCRS20/1401</t>
-  </si>
-  <si>
-    <t>BILL NO.MCCRS20/1400</t>
-  </si>
-  <si>
-    <t>BILL NO.MCCRS20/1403</t>
-  </si>
-  <si>
     <t>Sri Vimala Textiles, Vijayawada</t>
   </si>
   <si>
@@ -262,9 +244,6 @@
     <t>bill no.SWCRS20/543</t>
   </si>
   <si>
-    <t>BILL NO.MCCRS20/1430</t>
-  </si>
-  <si>
     <t>BILL NO.JCRS20/698</t>
   </si>
   <si>
@@ -310,9 +289,6 @@
     <t>BILL NO.24</t>
   </si>
   <si>
-    <t>BILL NO.MCCRS20/1454</t>
-  </si>
-  <si>
     <t>bill no.CRS20/1532</t>
   </si>
   <si>
@@ -337,9 +313,6 @@
     <t>BILL NO.BCRS20/689</t>
   </si>
   <si>
-    <t>BILL NO.MICRS20/404</t>
-  </si>
-  <si>
     <t>BILL NO.KCRS20/405</t>
   </si>
   <si>
@@ -415,12 +388,6 @@
     <t>BILL NO.TOCRS20/86</t>
   </si>
   <si>
-    <t>BILL NO.MCCRS20/1530</t>
-  </si>
-  <si>
-    <t>BILL NO.MICRS20/428</t>
-  </si>
-  <si>
     <t>bill no.158/20-21</t>
   </si>
   <si>
@@ -442,15 +409,6 @@
     <t>BILL NO.GST SALE 1106</t>
   </si>
   <si>
-    <t>BILL NO.MCCRS20/1603</t>
-  </si>
-  <si>
-    <t>BILL NO.MCCRS20/1594</t>
-  </si>
-  <si>
-    <t>BILL NO.MCCRS20/1595</t>
-  </si>
-  <si>
     <t>BILL NO.SOCRS20/393</t>
   </si>
   <si>
@@ -484,12 +442,6 @@
     <t>BILL NO.201100805 (5%)</t>
   </si>
   <si>
-    <t>BILL NO.M1CRS20/451</t>
-  </si>
-  <si>
-    <t>BILL NO.M1CRS20/452</t>
-  </si>
-  <si>
     <t>Kishore Fabrics Pvt Ltd., Vja</t>
   </si>
   <si>
@@ -569,12 +521,60 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201375</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201366</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201401</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201400</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201403</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201430</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201454</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201530</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201603</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201594</t>
+  </si>
+  <si>
+    <t>BILL NO.MCCRS201595</t>
+  </si>
+  <si>
+    <t>BILL NO.M1CRS20387</t>
+  </si>
+  <si>
+    <t>BILL NO.M1CRS20451</t>
+  </si>
+  <si>
+    <t>BILL NO.M1CRS20452</t>
+  </si>
+  <si>
+    <t>BILL NO.M1CRS20/404</t>
+  </si>
+  <si>
+    <t>BILL NO.M1CRS20/428</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;&quot;0.00"/>
@@ -1138,10 +1138,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1439,7 +1441,7 @@
         <v>31</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
       <c r="F9" s="21">
         <v>10016</v>
@@ -1476,7 +1478,7 @@
         <v>31</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
       <c r="F10" s="21">
         <v>15445</v>
@@ -1504,16 +1506,16 @@
         <v>44137</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="F11" s="21">
         <v>12688</v>
@@ -1550,7 +1552,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" s="21">
         <v>10023</v>
@@ -1578,16 +1580,16 @@
         <v>44138</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F13" s="21">
         <v>86460</v>
@@ -1615,16 +1617,16 @@
         <v>44138</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" s="21">
         <v>21121</v>
@@ -1652,16 +1654,16 @@
         <v>44138</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15" s="21">
         <v>56165</v>
@@ -1698,7 +1700,7 @@
         <v>31</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>41</v>
+        <v>178</v>
       </c>
       <c r="F16" s="21">
         <v>4801</v>
@@ -1735,7 +1737,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F17" s="21">
         <v>8605.06</v>
@@ -1772,7 +1774,7 @@
         <v>21</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F18" s="21">
         <v>11238.19</v>
@@ -1809,7 +1811,7 @@
         <v>24</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F19" s="21">
         <v>19357</v>
@@ -1846,7 +1848,7 @@
         <v>24</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F20" s="21">
         <v>29091</v>
@@ -1883,7 +1885,7 @@
         <v>24</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F21" s="21">
         <v>15911</v>
@@ -1920,7 +1922,7 @@
         <v>24</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F22" s="21">
         <v>2881</v>
@@ -1957,7 +1959,7 @@
         <v>24</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F23" s="21">
         <v>5683</v>
@@ -1994,7 +1996,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F24" s="21">
         <v>1012</v>
@@ -2031,7 +2033,7 @@
         <v>31</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="F25" s="21">
         <v>1751</v>
@@ -2068,7 +2070,7 @@
         <v>31</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
       <c r="F26" s="21">
         <v>1751</v>
@@ -2105,7 +2107,7 @@
         <v>31</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>52</v>
+        <v>171</v>
       </c>
       <c r="F27" s="21">
         <v>2228</v>
@@ -2133,16 +2135,16 @@
         <v>44140</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F28" s="21">
         <v>18922</v>
@@ -2170,16 +2172,16 @@
         <v>44140</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F29" s="21">
         <v>5974</v>
@@ -2207,16 +2209,16 @@
         <v>44140</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F30" s="21">
         <v>5513</v>
@@ -2244,16 +2246,16 @@
         <v>44140</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F31" s="21">
         <v>4995</v>
@@ -2281,16 +2283,16 @@
         <v>44140</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F32" s="21">
         <v>8835</v>
@@ -2327,7 +2329,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F33" s="21">
         <v>21550</v>
@@ -2364,7 +2366,7 @@
         <v>18</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F34" s="21">
         <v>19602</v>
@@ -2401,7 +2403,7 @@
         <v>18</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F35" s="21">
         <v>15342</v>
@@ -2429,16 +2431,16 @@
         <v>44141</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F36" s="21">
         <v>17122</v>
@@ -2466,16 +2468,16 @@
         <v>44141</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F37" s="21">
         <v>25328</v>
@@ -2503,16 +2505,16 @@
         <v>44141</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F38" s="21">
         <v>48873</v>
@@ -2540,16 +2542,16 @@
         <v>44142</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F39" s="21">
         <v>22003</v>
@@ -2577,16 +2579,16 @@
         <v>44142</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F40" s="21">
         <v>2098</v>
@@ -2623,7 +2625,7 @@
         <v>31</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="F41" s="21">
         <v>35489</v>
@@ -2660,7 +2662,7 @@
         <v>24</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F42" s="21">
         <v>1894</v>
@@ -2697,7 +2699,7 @@
         <v>24</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F43" s="21">
         <v>23932</v>
@@ -2725,16 +2727,16 @@
         <v>44144</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F44" s="21">
         <v>8537</v>
@@ -2762,16 +2764,16 @@
         <v>44144</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F45" s="21">
         <v>7114</v>
@@ -2799,16 +2801,16 @@
         <v>44144</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F46" s="21">
         <v>3734</v>
@@ -2836,16 +2838,16 @@
         <v>44145</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F47" s="21">
         <v>24570</v>
@@ -2871,16 +2873,16 @@
         <v>44145</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F48" s="21">
         <v>16832</v>
@@ -2908,16 +2910,16 @@
         <v>44145</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F49" s="21">
         <v>2100</v>
@@ -2943,16 +2945,16 @@
         <v>44145</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C50" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F50" s="21">
         <v>5382</v>
@@ -2989,7 +2991,7 @@
         <v>31</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>96</v>
+        <v>173</v>
       </c>
       <c r="F51" s="21">
         <v>9729</v>
@@ -3017,16 +3019,16 @@
         <v>44146</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F52" s="21">
         <v>8918</v>
@@ -3054,16 +3056,16 @@
         <v>44146</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F53" s="21">
         <v>48996</v>
@@ -3091,16 +3093,16 @@
         <v>44146</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F54" s="21">
         <v>3675</v>
@@ -3135,7 +3137,7 @@
         <v>24</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F55" s="21">
         <v>13187</v>
@@ -3172,7 +3174,7 @@
         <v>24</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F56" s="21">
         <v>18378</v>
@@ -3209,7 +3211,7 @@
         <v>24</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F57" s="21">
         <v>604</v>
@@ -3246,7 +3248,7 @@
         <v>31</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="F58" s="21">
         <v>598</v>
@@ -3283,7 +3285,7 @@
         <v>28</v>
       </c>
       <c r="E59" s="20" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F59" s="21">
         <v>27211</v>
@@ -3320,7 +3322,7 @@
         <v>28</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F60" s="21">
         <v>3225</v>
@@ -3357,7 +3359,7 @@
         <v>24</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F61" s="21">
         <v>27483</v>
@@ -3394,7 +3396,7 @@
         <v>24</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F62" s="21">
         <v>7578</v>
@@ -3431,7 +3433,7 @@
         <v>21</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F63" s="21">
         <v>9514.36</v>
@@ -3457,16 +3459,16 @@
         <v>44148</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C64" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F64" s="21">
         <v>1939</v>
@@ -3503,7 +3505,7 @@
         <v>21</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F65" s="21">
         <v>33605.32</v>
@@ -3531,16 +3533,16 @@
         <v>44151</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C66" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F66" s="21">
         <v>2620</v>
@@ -3568,16 +3570,16 @@
         <v>44151</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F67" s="21">
         <v>3712</v>
@@ -3614,7 +3616,7 @@
         <v>24</v>
       </c>
       <c r="E68" s="20" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F68" s="21">
         <v>9982</v>
@@ -3651,7 +3653,7 @@
         <v>24</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F69" s="21">
         <v>961</v>
@@ -3688,7 +3690,7 @@
         <v>28</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F70" s="21">
         <v>2796</v>
@@ -3716,16 +3718,16 @@
         <v>44151</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C71" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F71" s="21">
         <v>6573</v>
@@ -3762,7 +3764,7 @@
         <v>18</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F72" s="21">
         <v>23093</v>
@@ -3790,14 +3792,14 @@
         <v>44153</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C73" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="16"/>
       <c r="E73" s="20" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F73" s="21">
         <v>29211</v>
@@ -3827,16 +3829,16 @@
         <v>44154</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C74" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F74" s="21">
         <v>36346</v>
@@ -3864,16 +3866,16 @@
         <v>44154</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C75" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F75" s="21">
         <v>38832</v>
@@ -3901,16 +3903,16 @@
         <v>44154</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C76" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F76" s="21">
         <v>23045</v>
@@ -3938,16 +3940,16 @@
         <v>44154</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C77" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E77" s="20" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F77" s="21">
         <v>18857</v>
@@ -3975,16 +3977,16 @@
         <v>44154</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C78" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D78" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E78" s="20" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F78" s="21">
         <v>8904</v>
@@ -4021,7 +4023,7 @@
         <v>24</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F79" s="21">
         <v>11294</v>
@@ -4058,7 +4060,7 @@
         <v>24</v>
       </c>
       <c r="E80" s="20" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F80" s="21">
         <v>12060</v>
@@ -4095,7 +4097,7 @@
         <v>24</v>
       </c>
       <c r="E81" s="20" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F81" s="21">
         <v>13681</v>
@@ -4132,7 +4134,7 @@
         <v>28</v>
       </c>
       <c r="E82" s="20" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F82" s="21">
         <v>3796</v>
@@ -4169,7 +4171,7 @@
         <v>31</v>
       </c>
       <c r="E83" s="20" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="F83" s="21">
         <v>32132</v>
@@ -4206,7 +4208,7 @@
         <v>31</v>
       </c>
       <c r="E84" s="20" t="s">
-        <v>132</v>
+        <v>182</v>
       </c>
       <c r="F84" s="21">
         <v>5363</v>
@@ -4234,16 +4236,16 @@
         <v>44156</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C85" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F85" s="21">
         <v>8602</v>
@@ -4271,16 +4273,16 @@
         <v>44156</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C86" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E86" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F86" s="21">
         <v>21191</v>
@@ -4308,16 +4310,16 @@
         <v>44159</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C87" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E87" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F87" s="21">
         <v>25749</v>
@@ -4345,16 +4347,16 @@
         <v>44159</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C88" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E88" s="20" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F88" s="21">
         <v>70739</v>
@@ -4382,16 +4384,16 @@
         <v>44159</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C89" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E89" s="20" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F89" s="21">
         <v>14070</v>
@@ -4426,7 +4428,7 @@
         <v>31</v>
       </c>
       <c r="E90" s="20" t="s">
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="F90" s="21">
         <v>20986</v>
@@ -4463,7 +4465,7 @@
         <v>31</v>
       </c>
       <c r="E91" s="20" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="F91" s="21">
         <v>45505</v>
@@ -4500,7 +4502,7 @@
         <v>31</v>
       </c>
       <c r="E92" s="20" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="F92" s="21">
         <v>37523</v>
@@ -4537,7 +4539,7 @@
         <v>28</v>
       </c>
       <c r="E93" s="20" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F93" s="21">
         <v>3916</v>
@@ -4574,7 +4576,7 @@
         <v>24</v>
       </c>
       <c r="E94" s="20" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F94" s="21">
         <v>3732</v>
@@ -4611,7 +4613,7 @@
         <v>24</v>
       </c>
       <c r="E95" s="20" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F95" s="21">
         <v>36276</v>
@@ -4648,7 +4650,7 @@
         <v>24</v>
       </c>
       <c r="E96" s="20" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F96" s="21">
         <v>15951</v>
@@ -4685,7 +4687,7 @@
         <v>24</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="F97" s="21">
         <v>32984</v>
@@ -4713,16 +4715,16 @@
         <v>44160</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C98" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="F98" s="21">
         <v>3120</v>
@@ -4750,16 +4752,16 @@
         <v>44160</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C99" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="F99" s="21">
         <v>2016</v>
@@ -4794,7 +4796,7 @@
         <v>21</v>
       </c>
       <c r="E100" s="20" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F100" s="21">
         <v>9934</v>
@@ -4831,7 +4833,7 @@
         <v>21</v>
       </c>
       <c r="E101" s="20" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="F101" s="21">
         <v>2618</v>
@@ -4868,7 +4870,7 @@
         <v>31</v>
       </c>
       <c r="E102" s="20" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="F102" s="21">
         <v>45219</v>
@@ -4905,7 +4907,7 @@
         <v>31</v>
       </c>
       <c r="E103" s="20" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="F103" s="21">
         <v>3625</v>
@@ -4933,16 +4935,16 @@
         <v>44161</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C104" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="E104" s="20" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="F104" s="21">
         <v>5311</v>
@@ -4970,16 +4972,16 @@
         <v>44161</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C105" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E105" s="20" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="F105" s="21">
         <v>63231</v>
@@ -5014,7 +5016,7 @@
         <v>21</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="F106" s="21">
         <v>4722</v>
@@ -5051,7 +5053,7 @@
         <v>21</v>
       </c>
       <c r="E107" s="20" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="F107" s="21">
         <v>5947</v>
@@ -5079,16 +5081,16 @@
         <v>44162</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C108" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E108" s="20" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="F108" s="21">
         <v>21837</v>
@@ -5116,16 +5118,16 @@
         <v>44162</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C109" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D109" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E109" s="20" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F109" s="21">
         <v>35200</v>
@@ -5153,16 +5155,16 @@
         <v>44162</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C110" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D110" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E110" s="20" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F110" s="21">
         <v>48855</v>
@@ -5190,16 +5192,16 @@
         <v>44163</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C111" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D111" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E111" s="20" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="F111" s="21">
         <v>3885</v>
@@ -5225,16 +5227,16 @@
         <v>44163</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C112" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D112" s="16" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E112" s="20" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="F112" s="21">
         <v>10007</v>
@@ -5271,7 +5273,7 @@
         <v>21</v>
       </c>
       <c r="E113" s="20" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="F113" s="21">
         <v>819</v>
@@ -5308,7 +5310,7 @@
         <v>24</v>
       </c>
       <c r="E114" s="20" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="F114" s="21">
         <v>10770</v>
@@ -5345,7 +5347,7 @@
         <v>24</v>
       </c>
       <c r="E115" s="20" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="F115" s="21">
         <v>1652</v>
@@ -5373,16 +5375,16 @@
         <v>44165</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C116" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D116" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E116" s="20" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F116" s="21">
         <v>70161</v>
@@ -5417,7 +5419,7 @@
         <v>21</v>
       </c>
       <c r="E117" s="20" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="F117" s="21">
         <v>6889</v>
@@ -5454,7 +5456,7 @@
         <v>21</v>
       </c>
       <c r="E118" s="20" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="F118" s="21">
         <v>9599</v>
@@ -5482,16 +5484,16 @@
         <v>44165</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C119" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D119" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E119" s="20" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F119" s="21">
         <v>30383</v>
@@ -5519,16 +5521,16 @@
         <v>44165</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C120" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D120" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E120" s="20" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="F120" s="21">
         <v>23841</v>
@@ -5565,7 +5567,7 @@
         <v>24</v>
       </c>
       <c r="E121" s="20" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="F121" s="21">
         <v>6466</v>
@@ -5602,7 +5604,7 @@
         <v>24</v>
       </c>
       <c r="E122" s="20" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="F122" s="21">
         <v>611</v>
@@ -5630,16 +5632,16 @@
         <v>44165</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C123" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E123" s="20" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="F123" s="21">
         <v>40838</v>
@@ -5667,16 +5669,16 @@
         <v>44165</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C124" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E124" s="20" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="F124" s="21">
         <v>32857</v>
@@ -5704,16 +5706,16 @@
         <v>44165</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C125" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D125" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E125" s="20" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="F125" s="21">
         <v>7455</v>
@@ -5741,16 +5743,16 @@
         <v>44165</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C126" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D126" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E126" s="20" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="F126" s="21">
         <v>6040</v>
@@ -5778,16 +5780,16 @@
         <v>44165</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C127" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D127" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E127" s="20" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="F127" s="21">
         <v>8244</v>
@@ -5813,7 +5815,7 @@
     <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" s="25"/>
       <c r="B128" s="26" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>

</xml_diff>